<commit_message>
Working towards getting simulation blinded
</commit_message>
<xml_diff>
--- a/Images/MC/ToyRadialFieldScan/Configs.xlsx
+++ b/Images/MC/ToyRadialFieldScan/Configs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/Images/MC/ToyRadialFieldScan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA27442-A37E-9044-8B9D-033B13CCD6B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA792680-EE71-5D45-B672-582412CF5AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{6472D1E4-BE1D-3F4D-81A2-230F9F8783E2}"/>
+    <workbookView xWindow="-2980" yWindow="-19260" windowWidth="27320" windowHeight="17040" xr2:uid="{6472D1E4-BE1D-3F4D-81A2-230F9F8783E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
   <si>
     <t>Config</t>
   </si>
@@ -42,22 +42,41 @@
   </si>
   <si>
     <t>dBr [ppm]</t>
+  </si>
+  <si>
+    <t>dBr (fit)</t>
+  </si>
+  <si>
+    <t>dBr (truth)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -85,10 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,18 +423,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B780CD0-3CDB-F348-BE44-F08968C6A8D1}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="B7:C7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,63 +445,171 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.73670000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>0.33129999999999998</v>
+      </c>
+      <c r="H2">
+        <v>0.33150000000000002</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>0.33129999999999998</v>
+      </c>
+      <c r="L2">
+        <v>0.3196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1.1739999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>0.47</v>
+      </c>
+      <c r="H3">
+        <v>0.4728</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>0.44819999999999999</v>
+      </c>
+      <c r="L3">
+        <v>0.45100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2.5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.73750000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="H4">
+        <v>0.60050000000000003</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>0.47</v>
+      </c>
+      <c r="L4">
+        <v>0.4728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>5.5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.43149999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>0.44819999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="L5">
+        <v>0.60050000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>5.5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.68689999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>0.63660000000000005</v>
+      </c>
+      <c r="H6">
+        <v>0.622</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>0.63660000000000005</v>
+      </c>
+      <c r="L6">
+        <v>0.622</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -490,8 +619,280 @@
       <c r="C7" s="1">
         <v>0.43149999999999999</v>
       </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="H7">
+        <v>0.79020000000000001</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="L7">
+        <v>0.79020000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.99370000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f>6*4*20</f>
+        <v>480</v>
+      </c>
+      <c r="G11">
+        <f>6*4*15</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f>F11/60</f>
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <f>G11/60</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.32279999999999998</v>
+      </c>
+      <c r="H16" s="3">
+        <v>9.9220000000000002E-5</v>
+      </c>
+      <c r="I16">
+        <v>0.33150000000000002</v>
+      </c>
+      <c r="J16" s="3">
+        <v>6.9649999999999998E-3</v>
+      </c>
+      <c r="L16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <v>0.32279999999999998</v>
+      </c>
+      <c r="N16" s="2">
+        <v>9.9220000000000002E-5</v>
+      </c>
+      <c r="O16">
+        <v>0.33150000000000002</v>
+      </c>
+      <c r="P16">
+        <v>6.9649999999999998E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="H17" s="3">
+        <v>2.0579999999999999E-4</v>
+      </c>
+      <c r="I17">
+        <v>0.46050000000000002</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.03E-2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>0.40870000000000001</v>
+      </c>
+      <c r="N17">
+        <v>2.6039999999999999E-4</v>
+      </c>
+      <c r="O17">
+        <v>0.41220000000000001</v>
+      </c>
+      <c r="P17">
+        <v>9.2169999999999995E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.58160000000000001</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3.3199999999999999E-4</v>
+      </c>
+      <c r="I18">
+        <v>0.58479999999999999</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.308E-2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="N18">
+        <v>2.0579999999999999E-4</v>
+      </c>
+      <c r="O18">
+        <v>0.46050000000000002</v>
+      </c>
+      <c r="P18">
+        <v>1.03E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.40870000000000001</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2.6039999999999999E-4</v>
+      </c>
+      <c r="I19">
+        <v>0.41220000000000001</v>
+      </c>
+      <c r="J19" s="3">
+        <v>9.2169999999999995E-3</v>
+      </c>
+      <c r="L19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>0.58050000000000002</v>
+      </c>
+      <c r="N19">
+        <v>5.1159999999999997E-4</v>
+      </c>
+      <c r="O19">
+        <v>0.56310000000000004</v>
+      </c>
+      <c r="P19">
+        <v>1.259E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.58050000000000002</v>
+      </c>
+      <c r="H20" s="3">
+        <v>5.1159999999999997E-4</v>
+      </c>
+      <c r="I20">
+        <v>0.56310000000000004</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1.259E-2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <v>0.58160000000000001</v>
+      </c>
+      <c r="N20">
+        <v>3.3199999999999999E-4</v>
+      </c>
+      <c r="O20">
+        <v>0.58479999999999999</v>
+      </c>
+      <c r="P20">
+        <v>1.308E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="H21" s="3">
+        <v>8.2660000000000003E-4</v>
+      </c>
+      <c r="I21">
+        <v>0.71530000000000005</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="N21">
+        <v>8.2660000000000003E-4</v>
+      </c>
+      <c r="O21">
+        <v>0.71530000000000005</v>
+      </c>
+      <c r="P21">
+        <v>1.6E-2</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L15:P21">
+    <sortCondition ref="M15:M21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>